<commit_message>
Updates to Backlog, now includes refactoring
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 2/Sprint 2 Backlog.xlsx
+++ b/Documentation/Sprint 2/Sprint 2 Backlog.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="Status">Sheet1!$K$1:$K$3</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>Duration (Hours)</t>
   </si>
@@ -89,27 +89,9 @@
     <t>Research graph api's for java android</t>
   </si>
   <si>
-    <t>Test code with sets of data</t>
-  </si>
-  <si>
-    <t>Research how to collect historic data from yahoo api</t>
-  </si>
-  <si>
-    <t>Plan how to implement this feature</t>
-  </si>
-  <si>
-    <t>Code the feature</t>
-  </si>
-  <si>
-    <t>Thomas, Mark</t>
-  </si>
-  <si>
     <t>Member(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">3. Updates Views </t>
-  </si>
-  <si>
     <t>Totals:</t>
   </si>
   <si>
@@ -119,9 +101,6 @@
     <t>Sprint 2: Task Description</t>
   </si>
   <si>
-    <t>Learn how to use new library</t>
-  </si>
-  <si>
     <t>Make text smaller to fit on screen</t>
   </si>
   <si>
@@ -135,13 +114,85 @@
   </si>
   <si>
     <t>Adam, Peter</t>
+  </si>
+  <si>
+    <t>Plan how to collect historic data from yahoo api</t>
+  </si>
+  <si>
+    <t>Learn how to use new AndroidPlot library</t>
+  </si>
+  <si>
+    <t>Get library set up and running</t>
+  </si>
+  <si>
+    <t>Plot lines using the historic data</t>
+  </si>
+  <si>
+    <t>Adjust the aethetics of the graph widget</t>
+  </si>
+  <si>
+    <t>Create Spinners and populate with appropriate text</t>
+  </si>
+  <si>
+    <t>Create a graph widget and plot a simple graph</t>
+  </si>
+  <si>
+    <t>Test the spinners are altering the correct time periods</t>
+  </si>
+  <si>
+    <t>Test the spinners are altering the correct company shares</t>
+  </si>
+  <si>
+    <t>Test the graph is plotting lines relative to the time period and shares correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Updates Views </t>
+  </si>
+  <si>
+    <t>Create new tab for 'Graphs', and code to run the tab activity</t>
+  </si>
+  <si>
+    <t>Mark, Thomas</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Hamish, Adam</t>
+  </si>
+  <si>
+    <t>Victor, Mark</t>
+  </si>
+  <si>
+    <t>Peter, Adam</t>
+  </si>
+  <si>
+    <t>3. JUnit Testing + Refactoring</t>
+  </si>
+  <si>
+    <t>Identify code to be refactored</t>
+  </si>
+  <si>
+    <t>Refactor Feed Parser file</t>
+  </si>
+  <si>
+    <t>Refactor Graph Activity file</t>
+  </si>
+  <si>
+    <t>Refactor Rockets file</t>
+  </si>
+  <si>
+    <t>Refactor Alerts file</t>
+  </si>
+  <si>
+    <t>Peter, Adam, Hamish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -281,51 +332,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom style="medium">
@@ -360,7 +366,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -374,18 +380,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -401,9 +395,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,19 +404,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
@@ -437,9 +428,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -741,20 +751,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="51.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" style="1" customWidth="1"/>
@@ -763,22 +773,25 @@
     <col min="14" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-      <c r="J1"/>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="21">
+      <c r="A1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -787,80 +800,104 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="4"/>
-      <c r="J2"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="9"/>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="16"/>
-      <c r="J5"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" s="3">
         <v>1</v>
       </c>
@@ -873,22 +910,38 @@
       <c r="H6" s="3">
         <v>0</v>
       </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="23">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="E7" s="3">
         <v>1</v>
       </c>
@@ -901,12 +954,26 @@
       <c r="H7" s="3">
         <v>0</v>
       </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="23">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -914,9 +981,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="E8" s="3">
         <v>1</v>
       </c>
@@ -929,12 +998,26 @@
       <c r="H8" s="3">
         <v>0</v>
       </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="23">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -943,24 +1026,32 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="4"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="17"/>
-      <c r="J10"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I9" s="3"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -970,7 +1061,7 @@
       <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="3">
@@ -985,22 +1076,36 @@
       <c r="H11" s="3">
         <v>0</v>
       </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="23">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="3">
@@ -1015,12 +1120,26 @@
       <c r="H12" s="3">
         <v>0</v>
       </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="23">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
@@ -1030,7 +1149,7 @@
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="3">
@@ -1045,195 +1164,747 @@
       <c r="H13" s="3">
         <v>0</v>
       </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="23">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="23">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="23">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="23">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="23">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="3">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B19" s="3">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3</v>
+      </c>
+      <c r="J19" s="23">
+        <v>3</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="29"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2</v>
+      </c>
+      <c r="F26" s="3">
+        <v>2</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>2</v>
+      </c>
+      <c r="I26" s="3">
+        <v>2</v>
+      </c>
+      <c r="J26" s="3">
+        <v>2</v>
+      </c>
+      <c r="K26" s="3">
+        <v>2</v>
+      </c>
+      <c r="L26" s="3">
+        <v>2</v>
+      </c>
+      <c r="M26" s="3">
+        <v>2</v>
+      </c>
+      <c r="N26" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="3">
+        <v>3</v>
+      </c>
+      <c r="F27" s="3">
+        <v>3</v>
+      </c>
+      <c r="G27" s="3">
+        <v>3</v>
+      </c>
+      <c r="H27" s="3">
+        <v>3</v>
+      </c>
+      <c r="I27" s="3">
+        <v>3</v>
+      </c>
+      <c r="J27" s="3">
+        <v>3</v>
+      </c>
+      <c r="K27" s="3">
+        <v>3</v>
+      </c>
+      <c r="L27" s="3">
+        <v>3</v>
+      </c>
+      <c r="M27" s="3">
+        <v>3</v>
+      </c>
+      <c r="N27" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="3">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="3">
+        <v>3</v>
+      </c>
+      <c r="F28" s="3">
+        <v>3</v>
+      </c>
+      <c r="G28" s="3">
+        <v>3</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3</v>
+      </c>
+      <c r="I28" s="3">
+        <v>3</v>
+      </c>
+      <c r="J28" s="3">
+        <v>3</v>
+      </c>
+      <c r="K28" s="3">
+        <v>3</v>
+      </c>
+      <c r="L28" s="3">
+        <v>3</v>
+      </c>
+      <c r="M28" s="3">
+        <v>3</v>
+      </c>
+      <c r="N28" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1</v>
+      </c>
+      <c r="L29" s="3">
+        <v>1</v>
+      </c>
+      <c r="M29" s="3">
+        <v>1</v>
+      </c>
+      <c r="N29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15" thickBot="1">
+      <c r="A30" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="14">
+        <v>1</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="14">
+        <v>1</v>
+      </c>
+      <c r="F30" s="14">
+        <v>1</v>
+      </c>
+      <c r="G30" s="14">
+        <v>1</v>
+      </c>
+      <c r="H30" s="14">
+        <v>1</v>
+      </c>
+      <c r="I30" s="14">
+        <v>1</v>
+      </c>
+      <c r="J30" s="14">
+        <v>1</v>
+      </c>
+      <c r="K30" s="14">
+        <v>1</v>
+      </c>
+      <c r="L30" s="14">
+        <v>1</v>
+      </c>
+      <c r="M30" s="14">
+        <v>1</v>
+      </c>
+      <c r="N30" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="D32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="3">
+        <f>SUM(E6:E30)</f>
         <v>25</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="3">
-        <v>10</v>
-      </c>
-      <c r="F15" s="3">
-        <v>10</v>
-      </c>
-      <c r="G15" s="3">
-        <v>8</v>
-      </c>
-      <c r="H15" s="3">
-        <v>5</v>
-      </c>
-      <c r="I15" s="4">
-        <v>5</v>
-      </c>
-      <c r="J15"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="19">
-        <v>2</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="19">
-        <v>2</v>
-      </c>
-      <c r="F16" s="19">
-        <v>2</v>
-      </c>
-      <c r="G16" s="19">
-        <v>2</v>
-      </c>
-      <c r="H16" s="19">
-        <v>2</v>
-      </c>
-      <c r="I16" s="20">
-        <v>2</v>
-      </c>
-      <c r="J16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18"/>
-      <c r="J18"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="3">
-        <f>SUM(E6:E16)</f>
-        <v>18</v>
-      </c>
-      <c r="F19" s="3">
-        <f t="shared" ref="F19:I19" si="0">SUM(F6:F16)</f>
-        <v>15</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F32" s="3">
+        <f t="shared" ref="F32:N32" si="0">SUM(F6:F30)</f>
+        <v>22</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="H32" s="3">
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+      <c r="I32" s="3">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
+      </c>
+      <c r="K32" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H19" s="3">
+      <c r="L32" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I19" s="3">
+        <v>10</v>
+      </c>
+      <c r="M32" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J19"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J21"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J22"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J23"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J24"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
-      <c r="J27"/>
+        <v>10</v>
+      </c>
+      <c r="N32" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1243,7 +1914,7 @@
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="D3">
       <formula1>SUM(K1:K3)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17 D6:D8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23">
       <formula1>$K$3:$M$3</formula1>
     </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="D4:D5">
@@ -1251,6 +1922,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1260,20 +1932,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1281,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1289,7 +1961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1297,7 +1969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1305,17 +1977,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1331,12 +2003,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
updated sprint backlog 2
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 2/Sprint 2 Backlog.xlsx
+++ b/Documentation/Sprint 2/Sprint 2 Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="13180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
   <si>
     <t>Duration (Hours)</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Test the graph is plotting lines relative to the time period and shares correctly</t>
   </si>
   <si>
-    <t xml:space="preserve">2. Updates Views </t>
-  </si>
-  <si>
     <t>Create new tab for 'Graphs', and code to run the tab activity</t>
   </si>
   <si>
@@ -167,9 +164,6 @@
     <t>Peter, Adam</t>
   </si>
   <si>
-    <t>3. JUnit Testing + Refactoring</t>
-  </si>
-  <si>
     <t>Identify code to be refactored</t>
   </si>
   <si>
@@ -186,6 +180,72 @@
   </si>
   <si>
     <t>Peter, Adam, Hamish</t>
+  </si>
+  <si>
+    <t>3. Setting up Alerts</t>
+  </si>
+  <si>
+    <t>2. Generating Weekly, Montly &amp; Yearly Graph</t>
+  </si>
+  <si>
+    <t>Research UI elements to allow the user to change the alert</t>
+  </si>
+  <si>
+    <t>Insert Sliders</t>
+  </si>
+  <si>
+    <t>Get Sliders to update with correct value</t>
+  </si>
+  <si>
+    <t>Set AlertActivity to update every time a slider is changed.</t>
+  </si>
+  <si>
+    <t>Get Value from Sliders</t>
+  </si>
+  <si>
+    <t>4. Updating Shares as they happen</t>
+  </si>
+  <si>
+    <t>Correct the summary page so when the tab is clicked it updates the shares</t>
+  </si>
+  <si>
+    <t>5. JUnit Testing + Refactoring</t>
+  </si>
+  <si>
+    <t>Junit Testing: FeedParserTest</t>
+  </si>
+  <si>
+    <t>Junit Testing: FinanceTest</t>
+  </si>
+  <si>
+    <t>Junit Testing: StockManagerTest</t>
+  </si>
+  <si>
+    <t>This is based on the agreed upon user stories for sprint 2.</t>
+  </si>
+  <si>
+    <t>This is based on the user stories that were completed in sprint 2.</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 2: Final Value = 12</t>
+  </si>
+  <si>
+    <t>Sprint 2: Estimated Velocity = 3</t>
+  </si>
+  <si>
+    <t>Sprint 1: Velocity = 5</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -216,21 +276,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,23 +313,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -360,11 +406,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -383,25 +427,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -413,22 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -450,11 +467,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,6 +507,437 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> 2: Burndown Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$3:$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thurs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Thurs</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$44:$N$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="88784256"/>
+        <c:axId val="88876160"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="88784256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Weekdays</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88876160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88876160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Duration</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>(Hours)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88784256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Velocity</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Overview for Sprints</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$F$57:$F$58</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$57:$G$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="129833984"/>
+        <c:axId val="130200704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="129833984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="130200704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="130200704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Duration</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>(Days)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129833984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>882650</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -755,40 +1228,40 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="64.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="1" customWidth="1"/>
-    <col min="5" max="11" width="8.77734375" style="1"/>
-    <col min="12" max="13" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.77734375" style="1"/>
+    <col min="4" max="4" width="10.81640625" style="1" customWidth="1"/>
+    <col min="5" max="11" width="8.81640625" style="1"/>
+    <col min="12" max="13" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14">
@@ -801,53 +1274,53 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="23"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="14"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="22" t="s">
+      <c r="D3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="N3" s="19" t="s">
         <v>6</v>
       </c>
     </row>
@@ -861,29 +1334,29 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="26"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="11"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
@@ -895,7 +1368,7 @@
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="3">
@@ -913,7 +1386,7 @@
       <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="14">
         <v>0</v>
       </c>
       <c r="K6" s="3">
@@ -939,7 +1412,7 @@
       <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="3">
@@ -957,7 +1430,7 @@
       <c r="I7" s="3">
         <v>0</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="14">
         <v>0</v>
       </c>
       <c r="K7" s="3">
@@ -983,7 +1456,7 @@
       <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="3">
@@ -1001,7 +1474,7 @@
       <c r="I8" s="3">
         <v>0</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="14">
         <v>0</v>
       </c>
       <c r="K8" s="3">
@@ -1027,29 +1500,29 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="26"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="12"/>
+      <c r="A10" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
@@ -1061,7 +1534,7 @@
       <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="3">
@@ -1079,7 +1552,7 @@
       <c r="I11" s="3">
         <v>0</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="14">
         <v>0</v>
       </c>
       <c r="K11" s="3">
@@ -1105,7 +1578,7 @@
       <c r="C12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="3">
@@ -1123,7 +1596,7 @@
       <c r="I12" s="3">
         <v>0</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="14">
         <v>0</v>
       </c>
       <c r="K12" s="3">
@@ -1149,7 +1622,7 @@
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="3">
@@ -1167,7 +1640,7 @@
       <c r="I13" s="3">
         <v>0</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J13" s="14">
         <v>0</v>
       </c>
       <c r="K13" s="3">
@@ -1191,9 +1664,9 @@
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="3">
@@ -1211,7 +1684,7 @@
       <c r="I14" s="3">
         <v>0</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="14">
         <v>0</v>
       </c>
       <c r="K14" s="3">
@@ -1229,15 +1702,15 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="3">
         <v>0.5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="3">
@@ -1279,9 +1752,9 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="3">
@@ -1299,7 +1772,7 @@
       <c r="I16" s="3">
         <v>0</v>
       </c>
-      <c r="J16" s="23">
+      <c r="J16" s="14">
         <v>0</v>
       </c>
       <c r="K16" s="3">
@@ -1323,9 +1796,9 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="3">
@@ -1343,7 +1816,7 @@
       <c r="I17" s="3">
         <v>0</v>
       </c>
-      <c r="J17" s="23">
+      <c r="J17" s="14">
         <v>0</v>
       </c>
       <c r="K17" s="3">
@@ -1367,9 +1840,9 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="3">
@@ -1387,7 +1860,7 @@
       <c r="I18" s="3">
         <v>0</v>
       </c>
-      <c r="J18" s="23">
+      <c r="J18" s="14">
         <v>0</v>
       </c>
       <c r="K18" s="3">
@@ -1411,10 +1884,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>9</v>
+        <v>44</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E19" s="3">
         <v>3</v>
@@ -1431,7 +1904,7 @@
       <c r="I19" s="3">
         <v>3</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J19" s="14">
         <v>3</v>
       </c>
       <c r="K19" s="3">
@@ -1455,10 +1928,10 @@
         <v>0.5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E20" s="3">
         <v>0.5</v>
@@ -1499,10 +1972,10 @@
         <v>0.5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E21" s="3">
         <v>0.5</v>
@@ -1543,10 +2016,10 @@
         <v>0.5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E22" s="3">
         <v>0.5</v>
@@ -1580,330 +2053,828 @@
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="29"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="4"/>
+      <c r="A24" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="8"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="11"/>
+      <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="14">
+        <v>1</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="14">
+        <v>0</v>
+      </c>
+      <c r="F25" s="14">
+        <v>0</v>
+      </c>
+      <c r="G25" s="14">
+        <v>0</v>
+      </c>
+      <c r="H25" s="14">
+        <v>0</v>
+      </c>
+      <c r="I25" s="14">
+        <v>1</v>
+      </c>
+      <c r="J25" s="14">
+        <v>0</v>
+      </c>
+      <c r="K25" s="14">
+        <v>0</v>
+      </c>
+      <c r="L25" s="14">
+        <v>0</v>
+      </c>
+      <c r="M25" s="14">
+        <v>0</v>
+      </c>
+      <c r="N25" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="3">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="3">
-        <v>2</v>
-      </c>
-      <c r="F26" s="3">
-        <v>2</v>
-      </c>
-      <c r="G26" s="3">
-        <v>2</v>
-      </c>
-      <c r="H26" s="3">
-        <v>2</v>
-      </c>
-      <c r="I26" s="3">
-        <v>2</v>
-      </c>
-      <c r="J26" s="3">
-        <v>2</v>
-      </c>
-      <c r="K26" s="3">
-        <v>2</v>
-      </c>
-      <c r="L26" s="3">
-        <v>2</v>
-      </c>
-      <c r="M26" s="3">
-        <v>2</v>
-      </c>
-      <c r="N26" s="4">
-        <v>2</v>
+        <v>55</v>
+      </c>
+      <c r="B26" s="14">
+        <v>1</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="14">
+        <v>0</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0</v>
+      </c>
+      <c r="G26" s="14">
+        <v>0</v>
+      </c>
+      <c r="H26" s="14">
+        <v>0</v>
+      </c>
+      <c r="I26" s="14">
+        <v>0</v>
+      </c>
+      <c r="J26" s="14">
+        <v>1</v>
+      </c>
+      <c r="K26" s="14">
+        <v>0</v>
+      </c>
+      <c r="L26" s="14">
+        <v>0</v>
+      </c>
+      <c r="M26" s="14">
+        <v>0</v>
+      </c>
+      <c r="N26" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="3">
-        <v>3</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="3">
-        <v>3</v>
-      </c>
-      <c r="F27" s="3">
-        <v>3</v>
-      </c>
-      <c r="G27" s="3">
-        <v>3</v>
-      </c>
-      <c r="H27" s="3">
-        <v>3</v>
-      </c>
-      <c r="I27" s="3">
-        <v>3</v>
-      </c>
-      <c r="J27" s="3">
-        <v>3</v>
-      </c>
-      <c r="K27" s="3">
-        <v>3</v>
-      </c>
-      <c r="L27" s="3">
-        <v>3</v>
-      </c>
-      <c r="M27" s="3">
-        <v>3</v>
-      </c>
-      <c r="N27" s="4">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="B27" s="14">
+        <v>1</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="14">
+        <v>0</v>
+      </c>
+      <c r="F27" s="14">
+        <v>0</v>
+      </c>
+      <c r="G27" s="14">
+        <v>0</v>
+      </c>
+      <c r="H27" s="14">
+        <v>0</v>
+      </c>
+      <c r="I27" s="14">
+        <v>0</v>
+      </c>
+      <c r="J27" s="14">
+        <v>1</v>
+      </c>
+      <c r="K27" s="14">
+        <v>0</v>
+      </c>
+      <c r="L27" s="14">
+        <v>0</v>
+      </c>
+      <c r="M27" s="14">
+        <v>0</v>
+      </c>
+      <c r="N27" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="3">
-        <v>3</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="3">
-        <v>3</v>
-      </c>
-      <c r="F28" s="3">
-        <v>3</v>
-      </c>
-      <c r="G28" s="3">
-        <v>3</v>
-      </c>
-      <c r="H28" s="3">
-        <v>3</v>
-      </c>
-      <c r="I28" s="3">
-        <v>3</v>
-      </c>
-      <c r="J28" s="3">
-        <v>3</v>
-      </c>
-      <c r="K28" s="3">
-        <v>3</v>
-      </c>
-      <c r="L28" s="3">
-        <v>3</v>
-      </c>
-      <c r="M28" s="3">
-        <v>3</v>
-      </c>
-      <c r="N28" s="4">
-        <v>3</v>
+        <v>58</v>
+      </c>
+      <c r="B28" s="14">
+        <v>1</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="14">
+        <v>0</v>
+      </c>
+      <c r="F28" s="14">
+        <v>0</v>
+      </c>
+      <c r="G28" s="14">
+        <v>0</v>
+      </c>
+      <c r="H28" s="14">
+        <v>0</v>
+      </c>
+      <c r="I28" s="14">
+        <v>0</v>
+      </c>
+      <c r="J28" s="14">
+        <v>1</v>
+      </c>
+      <c r="K28" s="14">
+        <v>0</v>
+      </c>
+      <c r="L28" s="14">
+        <v>0</v>
+      </c>
+      <c r="M28" s="14">
+        <v>0</v>
+      </c>
+      <c r="N28" s="24">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="14">
+        <v>1</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0</v>
+      </c>
+      <c r="F29" s="14">
+        <v>0</v>
+      </c>
+      <c r="G29" s="14">
+        <v>0</v>
+      </c>
+      <c r="H29" s="14">
+        <v>0</v>
+      </c>
+      <c r="I29" s="14">
+        <v>0</v>
+      </c>
+      <c r="J29" s="14">
+        <v>0</v>
+      </c>
+      <c r="K29" s="14">
+        <v>1</v>
+      </c>
+      <c r="L29" s="14">
+        <v>0</v>
+      </c>
+      <c r="M29" s="14">
+        <v>0</v>
+      </c>
+      <c r="N29" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="20"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="8"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <v>2</v>
+      </c>
+      <c r="L32" s="3">
+        <v>0</v>
+      </c>
+      <c r="M32" s="3">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="8"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="3">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="3">
+        <v>2</v>
+      </c>
+      <c r="F35" s="3">
+        <v>2</v>
+      </c>
+      <c r="G35" s="3">
+        <v>2</v>
+      </c>
+      <c r="H35" s="3">
+        <v>2</v>
+      </c>
+      <c r="I35" s="3">
+        <v>2</v>
+      </c>
+      <c r="J35" s="3">
+        <v>2</v>
+      </c>
+      <c r="K35" s="3">
+        <v>2</v>
+      </c>
+      <c r="L35" s="3">
+        <v>2</v>
+      </c>
+      <c r="M35" s="3">
+        <v>2</v>
+      </c>
+      <c r="N35" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="3">
+        <v>3</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="3">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="21" t="s">
+      <c r="D36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="3">
+        <v>3</v>
+      </c>
+      <c r="F36" s="3">
+        <v>3</v>
+      </c>
+      <c r="G36" s="3">
+        <v>3</v>
+      </c>
+      <c r="H36" s="3">
+        <v>3</v>
+      </c>
+      <c r="I36" s="3">
+        <v>3</v>
+      </c>
+      <c r="J36" s="3">
+        <v>3</v>
+      </c>
+      <c r="K36" s="3">
+        <v>3</v>
+      </c>
+      <c r="L36" s="3">
+        <v>3</v>
+      </c>
+      <c r="M36" s="3">
+        <v>3</v>
+      </c>
+      <c r="N36" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="3">
+        <v>3</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="3">
+        <v>3</v>
+      </c>
+      <c r="F37" s="3">
+        <v>3</v>
+      </c>
+      <c r="G37" s="3">
+        <v>3</v>
+      </c>
+      <c r="H37" s="3">
+        <v>3</v>
+      </c>
+      <c r="I37" s="3">
+        <v>3</v>
+      </c>
+      <c r="J37" s="3">
+        <v>3</v>
+      </c>
+      <c r="K37" s="3">
+        <v>3</v>
+      </c>
+      <c r="L37" s="3">
+        <v>4</v>
+      </c>
+      <c r="M37" s="3">
+        <v>4</v>
+      </c>
+      <c r="N37" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3">
+        <v>1</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1</v>
+      </c>
+      <c r="J38" s="3">
+        <v>1</v>
+      </c>
+      <c r="K38" s="3">
+        <v>1</v>
+      </c>
+      <c r="L38" s="3">
+        <v>4</v>
+      </c>
+      <c r="M38" s="3">
+        <v>4</v>
+      </c>
+      <c r="N38" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1</v>
+      </c>
+      <c r="I39" s="3">
+        <v>1</v>
+      </c>
+      <c r="J39" s="3">
+        <v>1</v>
+      </c>
+      <c r="K39" s="3">
+        <v>1</v>
+      </c>
+      <c r="L39" s="3">
+        <v>1</v>
+      </c>
+      <c r="M39" s="3">
+        <v>1</v>
+      </c>
+      <c r="N39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="3">
         <v>8</v>
       </c>
-      <c r="E29" s="3">
-        <v>1</v>
-      </c>
-      <c r="F29" s="3">
-        <v>1</v>
-      </c>
-      <c r="G29" s="3">
-        <v>1</v>
-      </c>
-      <c r="H29" s="3">
-        <v>1</v>
-      </c>
-      <c r="I29" s="3">
-        <v>1</v>
-      </c>
-      <c r="J29" s="3">
-        <v>1</v>
-      </c>
-      <c r="K29" s="3">
-        <v>1</v>
-      </c>
-      <c r="L29" s="3">
-        <v>1</v>
-      </c>
-      <c r="M29" s="3">
-        <v>1</v>
-      </c>
-      <c r="N29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="15" thickBot="1">
-      <c r="A30" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="14">
-        <v>1</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="17" t="s">
+      <c r="C40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1</v>
+      </c>
+      <c r="J40" s="3">
+        <v>2</v>
+      </c>
+      <c r="K40" s="3">
+        <v>2</v>
+      </c>
+      <c r="L40" s="3">
+        <v>1</v>
+      </c>
+      <c r="M40" s="3">
+        <v>1</v>
+      </c>
+      <c r="N40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="3">
         <v>8</v>
       </c>
-      <c r="E30" s="14">
-        <v>1</v>
-      </c>
-      <c r="F30" s="14">
-        <v>1</v>
-      </c>
-      <c r="G30" s="14">
-        <v>1</v>
-      </c>
-      <c r="H30" s="14">
-        <v>1</v>
-      </c>
-      <c r="I30" s="14">
-        <v>1</v>
-      </c>
-      <c r="J30" s="14">
-        <v>1</v>
-      </c>
-      <c r="K30" s="14">
-        <v>1</v>
-      </c>
-      <c r="L30" s="14">
-        <v>1</v>
-      </c>
-      <c r="M30" s="14">
-        <v>1</v>
-      </c>
-      <c r="N30" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="D32" s="3" t="s">
+      <c r="C41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3">
+        <v>1</v>
+      </c>
+      <c r="H41" s="3">
+        <v>1</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1</v>
+      </c>
+      <c r="J41" s="3">
+        <v>2</v>
+      </c>
+      <c r="K41" s="3">
+        <v>2</v>
+      </c>
+      <c r="L41" s="3">
+        <v>1</v>
+      </c>
+      <c r="M41" s="3">
+        <v>0</v>
+      </c>
+      <c r="N41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15" thickBot="1">
+      <c r="A42" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="10">
+        <v>8</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="10">
+        <v>1</v>
+      </c>
+      <c r="F42" s="10">
+        <v>1</v>
+      </c>
+      <c r="G42" s="10">
+        <v>1</v>
+      </c>
+      <c r="H42" s="10">
+        <v>1</v>
+      </c>
+      <c r="I42" s="10">
+        <v>1</v>
+      </c>
+      <c r="J42" s="10">
+        <v>2</v>
+      </c>
+      <c r="K42" s="10">
+        <v>2</v>
+      </c>
+      <c r="L42" s="10">
+        <v>1</v>
+      </c>
+      <c r="M42" s="10">
+        <v>0</v>
+      </c>
+      <c r="N42" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="D44" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="3">
-        <f>SUM(E6:E30)</f>
+      <c r="E44" s="3">
+        <f>SUM(E6:E42)</f>
+        <v>28</v>
+      </c>
+      <c r="F44" s="3">
+        <f>SUM(F6:F42)</f>
         <v>25</v>
       </c>
-      <c r="F32" s="3">
-        <f t="shared" ref="F32:N32" si="0">SUM(F6:F30)</f>
-        <v>22</v>
-      </c>
-      <c r="G32" s="3">
-        <f t="shared" si="0"/>
-        <v>17.5</v>
-      </c>
-      <c r="H32" s="3">
-        <f t="shared" si="0"/>
-        <v>13.5</v>
-      </c>
-      <c r="I32" s="3">
-        <f t="shared" si="0"/>
-        <v>14.5</v>
-      </c>
-      <c r="J32" s="3">
-        <f t="shared" si="0"/>
-        <v>14.5</v>
-      </c>
-      <c r="K32" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L32" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M32" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="N32" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="G44" s="3">
+        <f>SUM(G6:G42)</f>
+        <v>20.5</v>
+      </c>
+      <c r="H44" s="3">
+        <f>SUM(H6:H42)</f>
+        <v>16.5</v>
+      </c>
+      <c r="I44" s="3">
+        <f>SUM(I6:I42)</f>
+        <v>18.5</v>
+      </c>
+      <c r="J44" s="3">
+        <f>SUM(J6:J42)</f>
+        <v>23.5</v>
+      </c>
+      <c r="K44" s="3">
+        <f>SUM(K6:K42)</f>
+        <v>19</v>
+      </c>
+      <c r="L44" s="3">
+        <f>SUM(L6:L42)</f>
+        <v>17</v>
+      </c>
+      <c r="M44" s="3">
+        <f>SUM(M6:M42)</f>
+        <v>15</v>
+      </c>
+      <c r="N44" s="3">
+        <f>SUM(N6:N42)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="6:7" ht="15.5">
+      <c r="F49" s="28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="6:7">
+      <c r="F50" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="6:7" ht="15.5">
+      <c r="F51" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="6:7">
+      <c r="F52" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="6:7" ht="15.5">
+      <c r="F54" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="6:7" ht="15" thickBot="1"/>
+    <row r="56" spans="6:7">
+      <c r="F56" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G56" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="6:7">
+      <c r="F57" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G57" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="6:7" ht="15" thickBot="1">
+      <c r="F58" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G58" s="11">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1914,7 +2885,7 @@
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="D3">
       <formula1>SUM(K1:K3)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23:D24 D30:D31">
       <formula1>$K$3:$M$3</formula1>
     </dataValidation>
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="D4:D5">
@@ -1923,6 +2894,7 @@
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1939,10 +2911,10 @@
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2008,7 +2980,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>